<commit_message>
Enhanced error handling a bit
</commit_message>
<xml_diff>
--- a/resources/Gehaltabrechnung.xlsx
+++ b/resources/Gehaltabrechnung.xlsx
@@ -36,259 +36,259 @@
     <t>Geburtsdatum</t>
   </si>
   <si>
+    <t>Tarif</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>Achen</t>
+  </si>
+  <si>
+    <t>Lukas</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Louisa</t>
+  </si>
+  <si>
+    <t>Markus</t>
+  </si>
+  <si>
+    <t>Adamek</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Adler</t>
+  </si>
+  <si>
+    <t>Mandy</t>
+  </si>
+  <si>
+    <t>Baier</t>
+  </si>
+  <si>
+    <t>Uwe</t>
+  </si>
+  <si>
+    <t>Beckenbauer</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Bürger</t>
+  </si>
+  <si>
+    <t>Petra</t>
+  </si>
+  <si>
+    <t>Daecher</t>
+  </si>
+  <si>
+    <t>Christina</t>
+  </si>
+  <si>
+    <t>Eisenberger</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Faubert</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Frankfurter</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Hopkins</t>
+  </si>
+  <si>
+    <t>Carl</t>
+  </si>
+  <si>
+    <t>Kaiser</t>
+  </si>
+  <si>
+    <t>Sabine</t>
+  </si>
+  <si>
+    <t>Kalowski</t>
+  </si>
+  <si>
+    <t>Stefan</t>
+  </si>
+  <si>
+    <t>Linus</t>
+  </si>
+  <si>
+    <t>Kilpeläinen</t>
+  </si>
+  <si>
+    <t>Henna</t>
+  </si>
+  <si>
+    <t>Kortig</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Maier</t>
+  </si>
+  <si>
+    <t>Matthias</t>
+  </si>
+  <si>
+    <t>Laurin</t>
+  </si>
+  <si>
+    <t>Maur</t>
+  </si>
+  <si>
+    <t>Claudia</t>
+  </si>
+  <si>
+    <t>Meier</t>
+  </si>
+  <si>
+    <t>Ede</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Meyer</t>
+  </si>
+  <si>
+    <t>Henri</t>
+  </si>
+  <si>
+    <t>Möller</t>
+  </si>
+  <si>
+    <t>Karsten</t>
+  </si>
+  <si>
+    <t>Morris</t>
+  </si>
+  <si>
+    <t>Vernon</t>
+  </si>
+  <si>
+    <t>Müller</t>
+  </si>
+  <si>
+    <t>Marc</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Nacht</t>
+  </si>
+  <si>
+    <t>Florian</t>
+  </si>
+  <si>
+    <t>Nagel</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Schiffer</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Schneider</t>
+  </si>
+  <si>
+    <t>Schröder</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Kerstin</t>
+  </si>
+  <si>
+    <t>Schultheiss</t>
+  </si>
+  <si>
+    <t>Maximilian</t>
+  </si>
+  <si>
+    <t>Schweizer</t>
+  </si>
+  <si>
+    <t>Ulrike</t>
+  </si>
+  <si>
+    <t>Sharpe</t>
+  </si>
+  <si>
+    <t>Nichole</t>
+  </si>
+  <si>
+    <t>Strauss</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>Theissen</t>
+  </si>
+  <si>
+    <t>Monika</t>
+  </si>
+  <si>
+    <t>Jahresgehalt</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
     <t>Monatsgehalt September</t>
-  </si>
-  <si>
-    <t>Tarif</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>AT</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>Achen</t>
-  </si>
-  <si>
-    <t>Lukas</t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>Louisa</t>
-  </si>
-  <si>
-    <t>Markus</t>
-  </si>
-  <si>
-    <t>Adamek</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Adler</t>
-  </si>
-  <si>
-    <t>Mandy</t>
-  </si>
-  <si>
-    <t>Baier</t>
-  </si>
-  <si>
-    <t>Uwe</t>
-  </si>
-  <si>
-    <t>Beckenbauer</t>
-  </si>
-  <si>
-    <t>Tim</t>
-  </si>
-  <si>
-    <t>Bürger</t>
-  </si>
-  <si>
-    <t>Petra</t>
-  </si>
-  <si>
-    <t>Daecher</t>
-  </si>
-  <si>
-    <t>Christina</t>
-  </si>
-  <si>
-    <t>Eisenberger</t>
-  </si>
-  <si>
-    <t>Sandra</t>
-  </si>
-  <si>
-    <t>Faubert</t>
-  </si>
-  <si>
-    <t>Anna</t>
-  </si>
-  <si>
-    <t>Frankfurter</t>
-  </si>
-  <si>
-    <t>Christian</t>
-  </si>
-  <si>
-    <t>Hopkins</t>
-  </si>
-  <si>
-    <t>Carl</t>
-  </si>
-  <si>
-    <t>Kaiser</t>
-  </si>
-  <si>
-    <t>Sabine</t>
-  </si>
-  <si>
-    <t>Kalowski</t>
-  </si>
-  <si>
-    <t>Stefan</t>
-  </si>
-  <si>
-    <t>Linus</t>
-  </si>
-  <si>
-    <t>Kilpeläinen</t>
-  </si>
-  <si>
-    <t>Henna</t>
-  </si>
-  <si>
-    <t>Kortig</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Maier</t>
-  </si>
-  <si>
-    <t>Matthias</t>
-  </si>
-  <si>
-    <t>Laurin</t>
-  </si>
-  <si>
-    <t>Maur</t>
-  </si>
-  <si>
-    <t>Claudia</t>
-  </si>
-  <si>
-    <t>Meier</t>
-  </si>
-  <si>
-    <t>Ede</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Meyer</t>
-  </si>
-  <si>
-    <t>Henri</t>
-  </si>
-  <si>
-    <t>Möller</t>
-  </si>
-  <si>
-    <t>Karsten</t>
-  </si>
-  <si>
-    <t>Morris</t>
-  </si>
-  <si>
-    <t>Vernon</t>
-  </si>
-  <si>
-    <t>Müller</t>
-  </si>
-  <si>
-    <t>Marc</t>
-  </si>
-  <si>
-    <t>Roger</t>
-  </si>
-  <si>
-    <t>Nacht</t>
-  </si>
-  <si>
-    <t>Florian</t>
-  </si>
-  <si>
-    <t>Nagel</t>
-  </si>
-  <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>Schiffer</t>
-  </si>
-  <si>
-    <t>Andrea</t>
-  </si>
-  <si>
-    <t>Schneider</t>
-  </si>
-  <si>
-    <t>Schröder</t>
-  </si>
-  <si>
-    <t>Michael</t>
-  </si>
-  <si>
-    <t>Kerstin</t>
-  </si>
-  <si>
-    <t>Schultheiss</t>
-  </si>
-  <si>
-    <t>Maximilian</t>
-  </si>
-  <si>
-    <t>Schweizer</t>
-  </si>
-  <si>
-    <t>Ulrike</t>
-  </si>
-  <si>
-    <t>Sharpe</t>
-  </si>
-  <si>
-    <t>Nichole</t>
-  </si>
-  <si>
-    <t>Strauss</t>
-  </si>
-  <si>
-    <t>Mario</t>
-  </si>
-  <si>
-    <t>Theissen</t>
-  </si>
-  <si>
-    <t>Monika</t>
-  </si>
-  <si>
-    <t>Jahresgehalt</t>
-  </si>
-  <si>
-    <t>Bonus</t>
-  </si>
-  <si>
-    <t>22</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,16 +658,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
@@ -675,10 +675,10 @@
         <v>127835</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="1">
         <v>21270</v>
@@ -687,7 +687,7 @@
         <v>5738.13</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2">
         <v>76030.222500000003</v>
@@ -701,10 +701,10 @@
         <v>127855</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
       </c>
       <c r="D3" s="1">
         <v>30014</v>
@@ -713,7 +713,7 @@
         <v>2978.45</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="2">
         <v>39464.462499999994</v>
@@ -727,10 +727,10 @@
         <v>127863</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <v>24605</v>
@@ -739,7 +739,7 @@
         <v>8532.7800000000007</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="2">
         <v>113059.33500000001</v>
@@ -753,10 +753,10 @@
         <v>127851</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="1">
         <v>28782</v>
@@ -765,7 +765,7 @@
         <v>4529.1899999999996</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2">
         <v>60011.767499999994</v>
@@ -779,10 +779,10 @@
         <v>127841</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="1">
         <v>23865</v>
@@ -791,7 +791,7 @@
         <v>3645</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="2">
         <v>48296.25</v>
@@ -805,10 +805,10 @@
         <v>127846</v>
       </c>
       <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
       </c>
       <c r="D7" s="1">
         <v>25761</v>
@@ -817,7 +817,7 @@
         <v>3987</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="2">
         <v>52827.75</v>
@@ -831,10 +831,10 @@
         <v>127836</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
       </c>
       <c r="D8" s="1">
         <v>21477</v>
@@ -843,7 +843,7 @@
         <v>4700.3</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="2">
         <v>62278.975000000006</v>
@@ -857,10 +857,10 @@
         <v>127867</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
       </c>
       <c r="D9" s="1">
         <v>34768</v>
@@ -869,7 +869,7 @@
         <v>2550.4</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" s="2">
         <v>33792.800000000003</v>
@@ -883,10 +883,10 @@
         <v>127834</v>
       </c>
       <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
       </c>
       <c r="D10" s="1">
         <v>20663</v>
@@ -895,7 +895,7 @@
         <v>4100.7</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="2">
         <v>54334.274999999994</v>
@@ -909,10 +909,10 @@
         <v>127838</v>
       </c>
       <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
       </c>
       <c r="D11" s="1">
         <v>21995</v>
@@ -921,7 +921,7 @@
         <v>3456.21</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="2">
         <v>45794.782500000001</v>
@@ -935,10 +935,10 @@
         <v>127861</v>
       </c>
       <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
       </c>
       <c r="D12" s="1">
         <v>31324</v>
@@ -947,7 +947,7 @@
         <v>3600</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2">
         <v>47700</v>
@@ -961,10 +961,10 @@
         <v>127870</v>
       </c>
       <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
       </c>
       <c r="D13" s="1">
         <v>36431</v>
@@ -973,7 +973,7 @@
         <v>1370.4</v>
       </c>
       <c r="F13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G13" s="2">
         <v>18157.800000000003</v>
@@ -987,10 +987,10 @@
         <v>127839</v>
       </c>
       <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
       </c>
       <c r="D14" s="1">
         <v>23209</v>
@@ -999,7 +999,7 @@
         <v>18439.830000000002</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" s="2">
         <v>237873.80700000003</v>
@@ -1013,10 +1013,10 @@
         <v>127862</v>
       </c>
       <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
         <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
       </c>
       <c r="D15" s="1">
         <v>31585</v>
@@ -1025,7 +1025,7 @@
         <v>3600</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="2">
         <v>47700</v>
@@ -1039,10 +1039,10 @@
         <v>127847</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1">
         <v>26633</v>
@@ -1051,7 +1051,7 @@
         <v>5257</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16" s="2">
         <v>69655.25</v>
@@ -1065,10 +1065,10 @@
         <v>127832</v>
       </c>
       <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
         <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
       </c>
       <c r="D17" s="1">
         <v>18842</v>
@@ -1077,7 +1077,7 @@
         <v>4630.1000000000004</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17" s="2">
         <v>61348.825000000004</v>
@@ -1091,10 +1091,10 @@
         <v>127859</v>
       </c>
       <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
         <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
       </c>
       <c r="D18" s="1">
         <v>30485</v>
@@ -1103,7 +1103,7 @@
         <v>4800</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18" s="2">
         <v>63600</v>
@@ -1117,10 +1117,10 @@
         <v>127843</v>
       </c>
       <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
         <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
       </c>
       <c r="D19" s="1">
         <v>24337</v>
@@ -1129,7 +1129,7 @@
         <v>4986.45</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G19" s="2">
         <v>66070.462499999994</v>
@@ -1143,10 +1143,10 @@
         <v>127865</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1">
         <v>36194</v>
@@ -1155,7 +1155,7 @@
         <v>1370.4</v>
       </c>
       <c r="F20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G20" s="2">
         <v>18157.800000000003</v>
@@ -1169,10 +1169,10 @@
         <v>127854</v>
       </c>
       <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" t="s">
-        <v>50</v>
       </c>
       <c r="D21" s="1">
         <v>29774</v>
@@ -1181,7 +1181,7 @@
         <v>7400</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" s="2">
         <v>95460</v>
@@ -1195,10 +1195,10 @@
         <v>127856</v>
       </c>
       <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
         <v>52</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
       </c>
       <c r="D22" s="1">
         <v>30223</v>
@@ -1207,7 +1207,7 @@
         <v>3700</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G22" s="2">
         <v>49025</v>
@@ -1221,10 +1221,10 @@
         <v>127845</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="1">
         <v>25226</v>
@@ -1233,7 +1233,7 @@
         <v>9430</v>
       </c>
       <c r="F23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="2">
         <v>121647</v>
@@ -1247,10 +1247,10 @@
         <v>127833</v>
       </c>
       <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
         <v>54</v>
-      </c>
-      <c r="C24" t="s">
-        <v>55</v>
       </c>
       <c r="D24" s="1">
         <v>19331</v>
@@ -1259,7 +1259,7 @@
         <v>5900.3</v>
       </c>
       <c r="F24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G24" s="2">
         <v>78178.975000000006</v>
@@ -1273,10 +1273,10 @@
         <v>127869</v>
       </c>
       <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
         <v>57</v>
-      </c>
-      <c r="C25" t="s">
-        <v>58</v>
       </c>
       <c r="D25" s="1">
         <v>37489</v>
@@ -1285,7 +1285,7 @@
         <v>980.5</v>
       </c>
       <c r="F25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G25" s="2">
         <v>12991.625</v>
@@ -1299,10 +1299,10 @@
         <v>127850</v>
       </c>
       <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
         <v>59</v>
-      </c>
-      <c r="C26" t="s">
-        <v>60</v>
       </c>
       <c r="D26" s="1">
         <v>28342</v>
@@ -1311,7 +1311,7 @@
         <v>3489.25</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G26" s="2">
         <v>46232.5625</v>
@@ -1325,10 +1325,10 @@
         <v>127860</v>
       </c>
       <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
         <v>61</v>
-      </c>
-      <c r="C27" t="s">
-        <v>62</v>
       </c>
       <c r="D27" s="1">
         <v>30788</v>
@@ -1337,7 +1337,7 @@
         <v>4500</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G27" s="2">
         <v>59625</v>
@@ -1351,10 +1351,10 @@
         <v>127866</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" s="1">
         <v>33865</v>
@@ -1363,7 +1363,7 @@
         <v>3200</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G28" s="2">
         <v>42400</v>
@@ -1377,10 +1377,10 @@
         <v>127842</v>
       </c>
       <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
         <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>64</v>
       </c>
       <c r="D29" s="1">
         <v>24024</v>
@@ -1389,7 +1389,7 @@
         <v>3978</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G29" s="2">
         <v>52708.5</v>
@@ -1403,10 +1403,10 @@
         <v>127871</v>
       </c>
       <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" t="s">
         <v>66</v>
-      </c>
-      <c r="C30" t="s">
-        <v>67</v>
       </c>
       <c r="D30" s="1">
         <v>35724</v>
@@ -1415,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G30" s="2">
         <v>20670</v>
@@ -1429,10 +1429,10 @@
         <v>127852</v>
       </c>
       <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
         <v>68</v>
-      </c>
-      <c r="C31" t="s">
-        <v>69</v>
       </c>
       <c r="D31" s="1">
         <v>28738</v>
@@ -1441,7 +1441,7 @@
         <v>4909.2299999999996</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G31" s="2">
         <v>65047.297499999993</v>
@@ -1455,10 +1455,10 @@
         <v>127848</v>
       </c>
       <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
         <v>70</v>
-      </c>
-      <c r="C32" t="s">
-        <v>71</v>
       </c>
       <c r="D32" s="1">
         <v>27014</v>
@@ -1467,7 +1467,7 @@
         <v>4245</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G32" s="2">
         <v>56246.25</v>
@@ -1481,10 +1481,10 @@
         <v>127857</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D33" s="1">
         <v>30254</v>
@@ -1493,7 +1493,7 @@
         <v>3256</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G33" s="2">
         <v>43142</v>
@@ -1507,10 +1507,10 @@
         <v>127853</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="1">
         <v>29164</v>
@@ -1519,7 +1519,7 @@
         <v>5200</v>
       </c>
       <c r="F34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G34" s="2">
         <v>68900</v>
@@ -1533,10 +1533,10 @@
         <v>127849</v>
       </c>
       <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
         <v>73</v>
-      </c>
-      <c r="C35" t="s">
-        <v>74</v>
       </c>
       <c r="D35" s="1">
         <v>27908</v>
@@ -1545,7 +1545,7 @@
         <v>4589.13</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G35" s="2">
         <v>60805.972500000003</v>
@@ -1559,10 +1559,10 @@
         <v>127844</v>
       </c>
       <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
         <v>73</v>
-      </c>
-      <c r="C36" t="s">
-        <v>74</v>
       </c>
       <c r="D36" s="1">
         <v>24697</v>
@@ -1571,7 +1571,7 @@
         <v>4908.45</v>
       </c>
       <c r="F36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G36" s="2">
         <v>65036.962499999994</v>
@@ -1585,10 +1585,10 @@
         <v>127840</v>
       </c>
       <c r="B37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
         <v>76</v>
-      </c>
-      <c r="C37" t="s">
-        <v>77</v>
       </c>
       <c r="D37" s="1">
         <v>23448</v>
@@ -1597,7 +1597,7 @@
         <v>10378.34</v>
       </c>
       <c r="F37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G37" s="2">
         <v>133880.58600000001</v>
@@ -1611,19 +1611,19 @@
         <v>127864</v>
       </c>
       <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" t="s">
         <v>78</v>
-      </c>
-      <c r="C38" t="s">
-        <v>79</v>
       </c>
       <c r="D38" s="1">
         <v>33547</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G38" s="2">
         <v>38425</v>
@@ -1637,10 +1637,10 @@
         <v>127868</v>
       </c>
       <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
         <v>80</v>
-      </c>
-      <c r="C39" t="s">
-        <v>81</v>
       </c>
       <c r="D39" s="1">
         <v>35856</v>
@@ -1649,7 +1649,7 @@
         <v>1560</v>
       </c>
       <c r="F39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G39" s="2">
         <v>20670</v>
@@ -1663,17 +1663,17 @@
         <v>127858</v>
       </c>
       <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" t="s">
         <v>82</v>
-      </c>
-      <c r="C40" t="s">
-        <v>83</v>
       </c>
       <c r="D40" s="1">
         <v>30433</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G40" s="2">
         <v>38425</v>
@@ -1687,10 +1687,10 @@
         <v>127837</v>
       </c>
       <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
         <v>84</v>
-      </c>
-      <c r="C41" t="s">
-        <v>85</v>
       </c>
       <c r="D41" s="1">
         <v>21693</v>
@@ -1699,7 +1699,7 @@
         <v>4320.45</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G41" s="2">
         <v>57245.962499999994</v>

</xml_diff>